<commit_message>
refactor: Add dynamic verification of topology objects and device types.
- Add new files and modify existing ones for improved functionality and debugging
- Implement support for parsing and generating device types and their ports
- Verify topology status using port verifiers and conjugate port verifiers
- Add new environment objective expression to the `compute` function in `ies_optim.py.j2`
- Replace print statements with logger calls in `type_def.py`
</commit_message>
<xml_diff>
--- a/microgrid_base/type_utils_resources/设备接口.xlsx
+++ b/microgrid_base/type_utils_resources/设备接口.xlsx
@@ -3882,7 +3882,7 @@
         <v>16</v>
       </c>
       <c r="G22" s="82" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="I22" s="82"/>
     </row>
@@ -3899,7 +3899,7 @@
         <v>16</v>
       </c>
       <c r="G23" s="82" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="I23" t="s">
         <v>37</v>

</xml_diff>